<commit_message>
Added MBA Staff data, Changed NSS, NCC, YRC json and function
</commit_message>
<xml_diff>
--- a/docs/STAFF-DATA/007.xlsx
+++ b/docs/STAFF-DATA/007.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Velammal-Engineering-College-Backend\docs\STAFF-DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{118979B5-E2AC-4842-B852-68BF2E589C1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2D4F5BE8-3785-4360-9547-812A36376C15}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
   </bookViews>
   <sheets>
     <sheet name="007" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="96">
   <si>
     <t>Name</t>
   </si>
@@ -305,12 +304,15 @@
   </si>
   <si>
     <t>VEC-007-04-117</t>
+  </si>
+  <si>
+    <t>Research Gate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1144,14 +1146,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E9EA39E-15D2-4D10-8F80-72E461EF40A5}">
-  <dimension ref="A1:I14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="57.21875" customWidth="1"/>
+    <col min="5" max="5" width="44.109375" customWidth="1"/>
+    <col min="6" max="6" width="31.6640625" customWidth="1"/>
+    <col min="7" max="7" width="20.44140625" customWidth="1"/>
+    <col min="8" max="8" width="22" customWidth="1"/>
+    <col min="9" max="9" width="25.21875" customWidth="1"/>
+    <col min="10" max="11" width="19" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1165,22 +1178,25 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1190,14 +1206,14 @@
       <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>12</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1210,20 +1226,20 @@
       <c r="D3" t="s">
         <v>16</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>17</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>18</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>19</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1236,23 +1252,23 @@
       <c r="D4" t="s">
         <v>23</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>24</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>25</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>26</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>27</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -1265,17 +1281,17 @@
       <c r="D5" t="s">
         <v>32</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>33</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>34</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>36</v>
       </c>
@@ -1288,23 +1304,23 @@
       <c r="D6" t="s">
         <v>38</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>39</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>40</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>41</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>42</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>44</v>
       </c>
@@ -1317,23 +1333,23 @@
       <c r="D7" t="s">
         <v>46</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>47</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>48</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>49</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>50</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>52</v>
       </c>
@@ -1343,14 +1359,14 @@
       <c r="C8" t="s">
         <v>53</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>54</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>56</v>
       </c>
@@ -1363,23 +1379,23 @@
       <c r="D9" t="s">
         <v>59</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>60</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>61</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>62</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>63</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>65</v>
       </c>
@@ -1392,20 +1408,20 @@
       <c r="D10" t="s">
         <v>68</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>69</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>18</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>70</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>72</v>
       </c>
@@ -1415,17 +1431,17 @@
       <c r="D11" t="s">
         <v>73</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>25</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>74</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>76</v>
       </c>
@@ -1438,14 +1454,14 @@
       <c r="D12" t="s">
         <v>78</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>79</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>81</v>
       </c>
@@ -1458,20 +1474,20 @@
       <c r="D13" t="s">
         <v>83</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>84</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>18</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>85</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>87</v>
       </c>
@@ -1484,19 +1500,19 @@
       <c r="D14" t="s">
         <v>89</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>90</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>91</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>92</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>93</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
         <v>94</v>
       </c>
     </row>

</xml_diff>